<commit_message>
Edits metadata to work twoards valid EML schema
</commit_message>
<xml_diff>
--- a/data-raw/metadata/F4F2019_ContinuousTempDO_AttributesTable.xlsx
+++ b/data-raw/metadata/F4F2019_ContinuousTempDO_AttributesTable.xlsx
@@ -1,40 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacobshikora\Documents\CalTrout\BORCharter\DataTransfer\2019Submission\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin Cain\Documents\Git\CVPIA\data-stewardship\EDI_data_repos_to_upload\fish-food-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{21FE8418-66A0-4594-B0A4-5CD3BBB24DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B94D742D-1EE6-4D6E-9A33-C6EC2FB31313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{17824303-BC38-4FFE-852F-26E788E3CF6F}"/>
+    <workbookView xWindow="20565" yWindow="-15975" windowWidth="15375" windowHeight="15225" xr2:uid="{17824303-BC38-4FFE-852F-26E788E3CF6F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="attribute" sheetId="1" r:id="rId1"/>
+    <sheet name="code_definitions" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
   <si>
     <t>dateTime</t>
   </si>
@@ -78,9 +70,6 @@
     <t>ratio</t>
   </si>
   <si>
-    <t>miligrams per liter</t>
-  </si>
-  <si>
     <t>dissolved oxygen of water at time of sample collection</t>
   </si>
   <si>
@@ -100,12 +89,6 @@
   </si>
   <si>
     <t>domain</t>
-  </si>
-  <si>
-    <t>definition</t>
-  </si>
-  <si>
-    <t>text_pattern</t>
   </si>
   <si>
     <t>type</t>
@@ -145,6 +128,18 @@
   </si>
   <si>
     <t>mm/dd/yyyy hh:mm</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>definitions</t>
+  </si>
+  <si>
+    <t>attribute_name</t>
+  </si>
+  <si>
+    <t>milligramPerLiter</t>
   </si>
 </sst>
 </file>
@@ -503,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93AC04F1-A5DF-4D2F-B22E-76D98ADCAD6B}">
-  <dimension ref="A1:AMJ8"/>
+  <dimension ref="A1:AMH8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,69 +512,61 @@
     <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.85546875" customWidth="1"/>
-    <col min="14" max="14" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.85546875" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1022" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>23</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>24</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>25</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>26</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>27</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>28</v>
       </c>
-      <c r="N1" t="s">
-        <v>29</v>
-      </c>
-      <c r="O1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P1" t="s">
-        <v>31</v>
-      </c>
     </row>
-    <row r="2" spans="1:1024" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1022" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -596,9 +583,7 @@
       <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -1614,12 +1599,10 @@
       <c r="AMF2" s="1"/>
       <c r="AMG2" s="1"/>
       <c r="AMH2" s="1"/>
-      <c r="AMI2" s="1"/>
-      <c r="AMJ2" s="1"/>
     </row>
-    <row r="3" spans="1:1024" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1022" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
@@ -1634,26 +1617,24 @@
       <c r="F3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O3" s="2">
+      <c r="K3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" s="2">
         <v>43517.520833333336</v>
       </c>
-      <c r="P3" s="3">
+      <c r="N3" s="3">
         <v>43564.4375</v>
       </c>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
@@ -2660,15 +2641,13 @@
       <c r="AMF3" s="1"/>
       <c r="AMG3" s="1"/>
       <c r="AMH3" s="1"/>
-      <c r="AMI3" s="1"/>
-      <c r="AMJ3" s="1"/>
     </row>
-    <row r="4" spans="1:1024" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1022" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>9</v>
@@ -2681,27 +2660,25 @@
         <v>11</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="I4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1">
+      <c r="M4" s="1">
         <v>0</v>
       </c>
-      <c r="P4" s="1">
+      <c r="N4" s="1">
         <v>20</v>
       </c>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
@@ -3708,12 +3685,10 @@
       <c r="AMF4" s="1"/>
       <c r="AMG4" s="1"/>
       <c r="AMH4" s="1"/>
-      <c r="AMI4" s="1"/>
-      <c r="AMJ4" s="1"/>
     </row>
-    <row r="5" spans="1:1024" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1022" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
@@ -3729,27 +3704,25 @@
         <v>11</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="I5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1">
+      <c r="M5" s="1">
         <v>0</v>
       </c>
-      <c r="P5" s="1">
+      <c r="N5" s="1">
         <v>30</v>
       </c>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
@@ -4756,24 +4729,22 @@
       <c r="AMF5" s="1"/>
       <c r="AMG5" s="1"/>
       <c r="AMH5" s="1"/>
-      <c r="AMI5" s="1"/>
-      <c r="AMJ5" s="1"/>
     </row>
-    <row r="6" spans="1:1024" ht="44.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:1024" ht="44.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:1024" ht="44.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:1022" ht="44.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:1022" ht="44.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:1022" ht="44.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4 D1:D5" xr:uid="{98F56C66-0433-45AA-A6A6-1BBFD0D43E73}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 D1:D5" xr:uid="{98F56C66-0433-45AA-A6A6-1BBFD0D43E73}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I3 I5" xr:uid="{474B035E-1DC0-4BD8-908F-B7F8CE50B162}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G3 G5" xr:uid="{474B035E-1DC0-4BD8-908F-B7F8CE50B162}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C5" xr:uid="{C1B84FFE-A77A-48CA-A8DF-8B9610109F8B}">
       <formula1>"string,boolean,decimal,float,double,duration,dateTime,time,date,gYearMonth,gYear,gMonthDay,gDay,gMonth"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K5" xr:uid="{E7FE37E6-B4A9-4B67-BF3C-4517507AE619}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I5" xr:uid="{E7FE37E6-B4A9-4B67-BF3C-4517507AE619}">
       <formula1>"natural,whole,interger,real"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F5" xr:uid="{8C657B0C-A4BE-4FDE-8FF4-6A3C836C8406}">
@@ -4782,4 +4753,30 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1EB56F0-22C8-4722-ADDF-34E09B0B7FDE}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>